<commit_message>
Ability modification part 1.
</commit_message>
<xml_diff>
--- a/xml/BGM.xlsx
+++ b/xml/BGM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Loop</t>
+  </si>
+  <si>
+    <t>Exceed the Sky</t>
+  </si>
+  <si>
+    <t>Junk Stereo Concept</t>
   </si>
 </sst>
 </file>
@@ -111,8 +117,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D5" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A2:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D7" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A2:D7"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="Name" name="Name">
       <xmlColumnPr mapId="1" xpath="/BGMs/BGM/Name" xmlDataType="string"/>
@@ -416,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -444,43 +450,71 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>21943</v>
       </c>
       <c r="C3">
-        <v>15000</v>
+        <v>21943</v>
       </c>
       <c r="D3">
-        <v>61875</v>
+        <v>61314</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>15360</v>
       </c>
       <c r="D4">
-        <v>42667</v>
+        <v>61440</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5">
+        <v>15000</v>
+      </c>
+      <c r="D5">
+        <v>61875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="D5">
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
         <v>28872</v>
       </c>
     </row>

</xml_diff>